<commit_message>
Remove the money fomat of the Amount field
</commit_message>
<xml_diff>
--- a/foo.xlsx
+++ b/foo.xlsx
@@ -44,10 +44,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-C0A];[RED]\-#,##0.00\ [$€-C0A]"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -123,7 +122,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,7 +146,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>